<commit_message>
docs: add missing sections for 2nd submissions
</commit_message>
<xml_diff>
--- a/capstone/report/statistics.xlsx
+++ b/capstone/report/statistics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="22">
   <si>
     <t>Algorithm</t>
   </si>
@@ -75,6 +75,25 @@
   </si>
   <si>
     <t>Performance Statistics</t>
+  </si>
+  <si>
+    <t>Maze</t>
+  </si>
+  <si>
+    <t>Optimal</t>
+  </si>
+  <si>
+    <t>Flood-Fill (no exploring)</t>
+  </si>
+  <si>
+    <t>Distance to center</t>
+  </si>
+  <si>
+    <t>Moves 
+(2nd round)</t>
+  </si>
+  <si>
+    <t>Score / Optimal Dist</t>
   </si>
 </sst>
 </file>
@@ -159,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -247,8 +266,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="34">
+  <cellStyleXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -283,8 +376,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -333,8 +430,59 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="34">
+  <cellStyles count="38">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -351,6 +499,8 @@
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -367,6 +517,8 @@
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -643,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H31"/>
+  <dimension ref="B2:Q31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:H31"/>
+      <selection activeCell="K4" sqref="K4:Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,19 +810,33 @@
     <col min="6" max="6" width="11" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="9" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="L4" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="27"/>
+      <c r="N4" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="33"/>
+      <c r="P4" s="27"/>
+    </row>
+    <row r="5" spans="2:17" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="C5" s="19" t="s">
         <v>0</v>
       </c>
@@ -689,8 +855,29 @@
       <c r="H5" s="21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -712,8 +899,30 @@
       <c r="H6" s="15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K6" s="22">
+        <v>1</v>
+      </c>
+      <c r="L6" s="28">
+        <v>30</v>
+      </c>
+      <c r="M6" s="15">
+        <v>17</v>
+      </c>
+      <c r="N6" s="14">
+        <v>34</v>
+      </c>
+      <c r="O6" s="14">
+        <v>18</v>
+      </c>
+      <c r="P6" s="34">
+        <v>21.03</v>
+      </c>
+      <c r="Q6" s="36">
+        <f>P6/L6</f>
+        <v>0.70100000000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7" s="6"/>
       <c r="C7" s="12" t="s">
         <v>3</v>
@@ -733,8 +942,30 @@
       <c r="H7" s="16">
         <v>29.067</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K7" s="23">
+        <v>2</v>
+      </c>
+      <c r="L7" s="29">
+        <v>43</v>
+      </c>
+      <c r="M7" s="30">
+        <v>23</v>
+      </c>
+      <c r="N7" s="7">
+        <v>43</v>
+      </c>
+      <c r="O7" s="7">
+        <v>25</v>
+      </c>
+      <c r="P7" s="16">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="37">
+        <f>P7/L7</f>
+        <v>0.76744186046511631</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" s="6"/>
       <c r="C8" s="12" t="s">
         <v>1</v>
@@ -754,8 +985,30 @@
       <c r="H8" s="16">
         <v>24.567</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K8" s="24">
+        <v>3</v>
+      </c>
+      <c r="L8" s="31">
+        <v>49</v>
+      </c>
+      <c r="M8" s="32">
+        <v>25</v>
+      </c>
+      <c r="N8" s="10">
+        <v>51</v>
+      </c>
+      <c r="O8" s="10">
+        <v>25</v>
+      </c>
+      <c r="P8" s="25">
+        <v>28.667000000000002</v>
+      </c>
+      <c r="Q8" s="38">
+        <f>P8/L8</f>
+        <v>0.5850408163265306</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
@@ -778,7 +1031,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B10" s="6"/>
       <c r="C10" s="12" t="s">
         <v>3</v>
@@ -799,7 +1052,7 @@
         <v>28.867000000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B11" s="9"/>
       <c r="C11" s="13" t="s">
         <v>1</v>
@@ -820,12 +1073,12 @@
         <v>21.03</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:17" ht="32" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
       <c r="C15" s="19" t="s">
         <v>0</v>
@@ -846,7 +1099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>9</v>
       </c>
@@ -1133,6 +1386,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:P4"/>
+  </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>